<commit_message>
Can vote but error pop up is wrong
</commit_message>
<xml_diff>
--- a/storage/app/excel/students.xlsx
+++ b/storage/app/excel/students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\07_Laravel\SchoolVoting\storage\app\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0271E723-07F5-4C7B-A96A-14A3A8C83C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2EED6A-85E2-4046-B2A0-D3151DEE94B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A361745D-60AC-400F-9ABF-9508250DE02D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t xml:space="preserve">BIST </t>
-  </si>
-  <si>
-    <t>7/30/2003</t>
   </si>
   <si>
     <t>Middle Name</t>
@@ -542,7 +539,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,7 +564,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -596,7 +593,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
@@ -729,7 +726,7 @@
         <v>9682481957</v>
       </c>
       <c r="I6" s="4">
-        <v>45463</v>
+        <v>38158</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -740,7 +737,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>27</v>
@@ -757,8 +754,8 @@
       <c r="H7" s="2">
         <v>9581928299</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>30</v>
+      <c r="I7" s="4">
+        <v>38198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
File upload still problem
</commit_message>
<xml_diff>
--- a/storage/app/excel/students.xlsx
+++ b/storage/app/excel/students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\07_Laravel\SchoolVoting\storage\app\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2EED6A-85E2-4046-B2A0-D3151DEE94B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81A3795-8212-4E71-92ED-2F4BA034C99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A361745D-60AC-400F-9ABF-9508250DE02D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>Camillo</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
@@ -539,7 +548,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,7 +561,8 @@
     <col min="6" max="7" width="8.88671875" style="2"/>
     <col min="8" max="8" width="16.21875" style="2" customWidth="1"/>
     <col min="9" max="9" width="24.6640625" style="2" customWidth="1"/>
-    <col min="10" max="11" width="8.88671875" style="2"/>
+    <col min="10" max="10" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="2"/>
     <col min="15" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
@@ -584,6 +594,9 @@
       <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
@@ -613,6 +626,9 @@
       <c r="I2" s="4">
         <f>DATE(2004,7,7)</f>
         <v>38175</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -647,6 +663,9 @@
         <f>DATE(2004,8,22)</f>
         <v>38221</v>
       </c>
+      <c r="J3" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
@@ -671,7 +690,11 @@
         <v>9571028591</v>
       </c>
       <c r="I4" s="4">
+        <f>DATE(2004,9,22)</f>
         <v>38252</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -697,7 +720,11 @@
         <v>9571822858</v>
       </c>
       <c r="I5" s="4">
+        <f>DATE(2005,1,19)</f>
         <v>38371</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -726,7 +753,11 @@
         <v>9682481957</v>
       </c>
       <c r="I6" s="4">
+        <f>DATE(2004,6,20)</f>
         <v>38158</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -755,7 +786,11 @@
         <v>9581928299</v>
       </c>
       <c r="I7" s="4">
-        <v>38198</v>
+        <f>DATE(2003,7,30)</f>
+        <v>37832</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Populated Results table but no UI yet
</commit_message>
<xml_diff>
--- a/storage/app/excel/students.xlsx
+++ b/storage/app/excel/students.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="0p15ogLtK4Kf+oNVIceT52nx77CgumoS34iDRgsJppY="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="5XQH+JA+7mkS/bbDfquHUDakRjvmF/sQt5+Us1RMeFE="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="167">
   <si>
     <t>ID</t>
   </si>
@@ -141,6 +141,18 @@
     <t>BSCS</t>
   </si>
   <si>
+    <t>Shane Claire</t>
+  </si>
+  <si>
+    <t>Galdiano</t>
+  </si>
+  <si>
+    <t>Beriong</t>
+  </si>
+  <si>
+    <t>s.beriong.544146@umindanao.edu.ph</t>
+  </si>
+  <si>
     <t>Lebron James</t>
   </si>
   <si>
@@ -254,12 +266,268 @@
   <si>
     <t>b.jackson.551239@umindanao.edu.ph</t>
   </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>Dominic</t>
+  </si>
+  <si>
+    <t>Villanueva</t>
+  </si>
+  <si>
+    <t>a.villanueva.556100@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Beatrice</t>
+  </si>
+  <si>
+    <t>Santos</t>
+  </si>
+  <si>
+    <t>b.santos.556101@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Manuel</t>
+  </si>
+  <si>
+    <t>Rivera</t>
+  </si>
+  <si>
+    <t>c.rivera.556102@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Denise</t>
+  </si>
+  <si>
+    <t>Rojas</t>
+  </si>
+  <si>
+    <t>d.rojas.556103@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>BMA</t>
+  </si>
+  <si>
+    <t>Elijah</t>
+  </si>
+  <si>
+    <t>Patricio</t>
+  </si>
+  <si>
+    <t>Cruz</t>
+  </si>
+  <si>
+    <t>e.cruz.556104@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Faith</t>
+  </si>
+  <si>
+    <t>Lim</t>
+  </si>
+  <si>
+    <t>f.lim.556105@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>Tomas</t>
+  </si>
+  <si>
+    <t>Morales</t>
+  </si>
+  <si>
+    <t>g.morales.556106@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Hannah</t>
+  </si>
+  <si>
+    <t>Reyes</t>
+  </si>
+  <si>
+    <t>h.reyes.556107@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Ian</t>
+  </si>
+  <si>
+    <t>Delos Reyes</t>
+  </si>
+  <si>
+    <t>i.delosreyes.556108@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Joy</t>
+  </si>
+  <si>
+    <t>Uy</t>
+  </si>
+  <si>
+    <t>Fernandez</t>
+  </si>
+  <si>
+    <t>j.fernandez.556109@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Andrea Marie</t>
+  </si>
+  <si>
+    <t>Samuel</t>
+  </si>
+  <si>
+    <t>Vaughn</t>
+  </si>
+  <si>
+    <t>a.vaughn.523746@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Joshua</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Domingo</t>
+  </si>
+  <si>
+    <t>j.domingo.545391@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Marian</t>
+  </si>
+  <si>
+    <t>Renato</t>
+  </si>
+  <si>
+    <t>m.cruza.534812@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Lianne</t>
+  </si>
+  <si>
+    <t>Anjali</t>
+  </si>
+  <si>
+    <t>Ricardo</t>
+  </si>
+  <si>
+    <t>l.ricardo.554099@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Siti</t>
+  </si>
+  <si>
+    <t>Ayesha</t>
+  </si>
+  <si>
+    <t>Ibrahim</t>
+  </si>
+  <si>
+    <t>s.ibrahim.521763@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Mateo Zander</t>
+  </si>
+  <si>
+    <t>Daiki</t>
+  </si>
+  <si>
+    <t>Kimura</t>
+  </si>
+  <si>
+    <t>m.kimura.525390@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>Mei</t>
+  </si>
+  <si>
+    <t>Zhang</t>
+  </si>
+  <si>
+    <t>p.zhang.534218@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Raj Luis</t>
+  </si>
+  <si>
+    <t>Saanvi</t>
+  </si>
+  <si>
+    <t>Neha</t>
+  </si>
+  <si>
+    <t>r.neha.522647@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>BSCSE</t>
+  </si>
+  <si>
+    <t>Karan</t>
+  </si>
+  <si>
+    <t>Ritesh</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>k.garcia.541837@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Vivek Kaito</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
+    <t>Enrique</t>
+  </si>
+  <si>
+    <t>v.enrique.525390@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Benedic </t>
+  </si>
+  <si>
+    <t>Fuentes</t>
+  </si>
+  <si>
+    <t>Dutaro</t>
+  </si>
+  <si>
+    <t>j.dutaro.545524@umindanao.edu.ph</t>
+  </si>
+  <si>
+    <t>Russel</t>
+  </si>
+  <si>
+    <t>Momblanco</t>
+  </si>
+  <si>
+    <t>Labiaga</t>
+  </si>
+  <si>
+    <t>r.labiaga.543519@umindanao.edu.ph</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -290,6 +558,10 @@
     </font>
     <font>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -308,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -327,11 +599,23 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,7 +1078,7 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="2">
+      <c r="A6" s="5">
         <v>545648.0</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -933,17 +1217,19 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="5">
-        <v>543429.0</v>
+        <v>544146.0</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="D9" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>14</v>
@@ -952,14 +1238,14 @@
         <v>2.0</v>
       </c>
       <c r="H9" s="5">
-        <v>9.457095887E9</v>
+        <v>9.77702619E9</v>
       </c>
       <c r="I9" s="6">
-        <f>DATE(2004,1,26)</f>
-        <v>38012</v>
+        <f>DATE(2005,1,28)</f>
+        <v>38380</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="K9" s="2"/>
       <c r="O9" s="2"/>
@@ -977,14 +1263,12 @@
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="5">
-        <v>529899.0</v>
+        <v>543429.0</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="5" t="s">
         <v>46</v>
       </c>
@@ -998,11 +1282,11 @@
         <v>2.0</v>
       </c>
       <c r="H10" s="5">
-        <v>9.922000788E9</v>
-      </c>
-      <c r="I10" s="6">
-        <f>DATE(2003,1,26)</f>
-        <v>37647</v>
+        <v>9.457095887E9</v>
+      </c>
+      <c r="I10" s="7">
+        <f>DATE(2004,1,26)</f>
+        <v>38012</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>15</v>
@@ -1023,7 +1307,7 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="5">
-        <v>541245.0</v>
+        <v>529899.0</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>48</v>
@@ -1038,17 +1322,17 @@
         <v>51</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="G11" s="5">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H11" s="5">
-        <v>9.602461153E9</v>
-      </c>
-      <c r="I11" s="6">
-        <f>DATE(2003,3,20)</f>
-        <v>37700</v>
+        <v>9.922000788E9</v>
+      </c>
+      <c r="I11" s="7">
+        <f>DATE(2003,1,26)</f>
+        <v>37647</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>15</v>
@@ -1069,30 +1353,32 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="5">
-        <v>531241.0</v>
+        <v>541245.0</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="D12" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="G12" s="5">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H12" s="5">
-        <v>9.531241412E9</v>
-      </c>
-      <c r="I12" s="6">
-        <f t="shared" ref="I12:I13" si="1">DATE(2002,1,26)</f>
-        <v>37282</v>
+        <v>9.602461153E9</v>
+      </c>
+      <c r="I12" s="7">
+        <f>DATE(2003,3,20)</f>
+        <v>37700</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>15</v>
@@ -1113,7 +1399,7 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="5">
-        <v>531123.0</v>
+        <v>531241.0</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>56</v>
@@ -1126,20 +1412,20 @@
         <v>58</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="G13" s="5">
         <v>4.0</v>
       </c>
       <c r="H13" s="5">
-        <v>9.514512311E9</v>
-      </c>
-      <c r="I13" s="6">
-        <f t="shared" si="1"/>
+        <v>9.531241412E9</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" ref="I13:I14" si="1">DATE(2002,1,26)</f>
         <v>37282</v>
       </c>
-      <c r="J13" s="4" t="s">
-        <v>23</v>
+      <c r="J13" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="K13" s="2"/>
       <c r="O13" s="2"/>
@@ -1157,30 +1443,30 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="5">
-        <v>543145.0</v>
+        <v>531123.0</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>40</v>
       </c>
       <c r="G14" s="5">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H14" s="5">
-        <v>9.814981329E9</v>
-      </c>
-      <c r="I14" s="6">
-        <f>DATE(2003,3,20)</f>
-        <v>37700</v>
+        <v>9.514512311E9</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="1"/>
+        <v>37282</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>23</v>
@@ -1201,30 +1487,30 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="5">
-        <v>531245.0</v>
+        <v>543145.0</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>40</v>
       </c>
       <c r="G15" s="5">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H15" s="5">
-        <v>9.372149192E9</v>
-      </c>
-      <c r="I15" s="6">
-        <f>DATE(2002,1,26)</f>
-        <v>37282</v>
+        <v>9.814981329E9</v>
+      </c>
+      <c r="I15" s="7">
+        <f>DATE(2003,3,20)</f>
+        <v>37700</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>23</v>
@@ -1245,30 +1531,30 @@
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="5">
-        <v>531244.0</v>
+        <v>531245.0</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>40</v>
       </c>
       <c r="G16" s="5">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H16" s="5">
-        <v>9.372184129E9</v>
-      </c>
-      <c r="I16" s="6">
-        <f>DATE(2003,3,20)</f>
-        <v>37700</v>
+        <v>9.372149192E9</v>
+      </c>
+      <c r="I16" s="7">
+        <f>DATE(2002,1,26)</f>
+        <v>37282</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>23</v>
@@ -1289,33 +1575,33 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="5">
-        <v>512344.0</v>
+        <v>531244.0</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>40</v>
       </c>
       <c r="G17" s="5">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H17" s="5">
-        <v>9.743184721E9</v>
-      </c>
-      <c r="I17" s="6">
-        <f>DATE(2002,1,26)</f>
-        <v>37282</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>15</v>
+        <v>9.372184129E9</v>
+      </c>
+      <c r="I17" s="7">
+        <f>DATE(2003,3,20)</f>
+        <v>37700</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="K17" s="2"/>
       <c r="O17" s="2"/>
@@ -1333,30 +1619,30 @@
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="5">
-        <v>554432.0</v>
+        <v>512344.0</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>40</v>
       </c>
       <c r="G18" s="5">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H18" s="5">
-        <v>9.382147817E9</v>
-      </c>
-      <c r="I18" s="6">
-        <f t="shared" ref="I18:I20" si="2">DATE(2003,3,20)</f>
-        <v>37700</v>
+        <v>9.743184721E9</v>
+      </c>
+      <c r="I18" s="7">
+        <f>DATE(2002,1,26)</f>
+        <v>37282</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>15</v>
@@ -1377,17 +1663,17 @@
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="5">
-        <v>561980.0</v>
+        <v>554432.0</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>40</v>
@@ -1396,10 +1682,10 @@
         <v>3.0</v>
       </c>
       <c r="H19" s="5">
-        <v>9.321658127E9</v>
-      </c>
-      <c r="I19" s="6">
-        <f t="shared" si="2"/>
+        <v>9.382147817E9</v>
+      </c>
+      <c r="I19" s="7">
+        <f t="shared" ref="I19:I21" si="2">DATE(2003,3,20)</f>
         <v>37700</v>
       </c>
       <c r="J19" s="5" t="s">
@@ -1421,17 +1707,17 @@
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="5">
-        <v>551239.0</v>
+        <v>561980.0</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>40</v>
@@ -1440,9 +1726,9 @@
         <v>3.0</v>
       </c>
       <c r="H20" s="5">
-        <v>9.571845147E9</v>
-      </c>
-      <c r="I20" s="6">
+        <v>9.321658127E9</v>
+      </c>
+      <c r="I20" s="7">
         <f t="shared" si="2"/>
         <v>37700</v>
       </c>
@@ -1464,16 +1750,35 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="5">
+        <v>551239.0</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="2"/>
+      <c r="D21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="H21" s="5">
+        <v>9.571845147E9</v>
+      </c>
+      <c r="I21" s="7">
+        <f t="shared" si="2"/>
+        <v>37700</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="K21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
@@ -1489,16 +1794,37 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="A22" s="8">
+        <v>556100.0</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="H22" s="8">
+        <v>9.601112233E9</v>
+      </c>
+      <c r="I22" s="9">
+        <f>DATE(2002,2,17)</f>
+        <v>37304</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="K22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
@@ -1514,16 +1840,35 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+      <c r="A23" s="8">
+        <v>556101.0</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="H23" s="8">
+        <v>9.612223344E9</v>
+      </c>
+      <c r="I23" s="9">
+        <f>DATE(2001,11,5)</f>
+        <v>37200</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="K23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -1539,16 +1884,37 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
+      <c r="A24" s="8">
+        <v>556102.0</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="H24" s="8">
+        <v>9.623334455E9</v>
+      </c>
+      <c r="I24" s="9">
+        <f>DATE(2002,6,23)</f>
+        <v>37430</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="K24" s="2"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
@@ -1564,16 +1930,35 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="A25" s="8">
+        <v>556103.0</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="H25" s="8">
+        <v>9.634445566E9</v>
+      </c>
+      <c r="I25" s="9">
+        <f>DATE(2001,8,19)</f>
+        <v>37122</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="K25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
@@ -1589,16 +1974,37 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
+      <c r="A26" s="5">
+        <v>556104.0</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="H26" s="8">
+        <v>9.645556677E9</v>
+      </c>
+      <c r="I26" s="9">
+        <f>DATE(2002,3,3)</f>
+        <v>37318</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="K26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
@@ -1614,16 +2020,35 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
+      <c r="A27" s="8">
+        <v>556105.0</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="H27" s="8">
+        <v>9.656667788E9</v>
+      </c>
+      <c r="I27" s="9">
+        <f>DATE(2001,12,29)</f>
+        <v>37254</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="K27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
@@ -1639,16 +2064,37 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
+      <c r="A28" s="8">
+        <v>556106.0</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="H28" s="8">
+        <v>9.667778899E9</v>
+      </c>
+      <c r="I28" s="9">
+        <f>DATE(2002,5,14)</f>
+        <v>37390</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="K28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
@@ -1664,16 +2110,35 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
+      <c r="A29" s="5">
+        <v>556107.0</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G29" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="H29" s="8">
+        <v>9.6788899E9</v>
+      </c>
+      <c r="I29" s="9">
+        <f>DATE(2002,1,8)</f>
+        <v>37264</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="K29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
@@ -1689,16 +2154,35 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
+      <c r="A30" s="8">
+        <v>556108.0</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="H30" s="8">
+        <v>9.689990011E9</v>
+      </c>
+      <c r="I30" s="9">
+        <f>DATE(2001,4,26)</f>
+        <v>37007</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="K30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
@@ -1714,16 +2198,37 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
+      <c r="A31" s="8">
+        <v>556109.0</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G31" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="H31" s="8">
+        <v>9.690001122E9</v>
+      </c>
+      <c r="I31" s="9">
+        <f>DATE(2001,9,15)</f>
+        <v>37149</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="K31" s="2"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
@@ -1739,16 +2244,37 @@
       <c r="Z31" s="2"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
+      <c r="A32" s="5">
+        <v>523746.0</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="H32" s="5">
+        <v>9.123456702E9</v>
+      </c>
+      <c r="I32" s="10">
+        <f>DATE(2003,11,4)</f>
+        <v>37929</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="K32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
@@ -1764,16 +2290,37 @@
       <c r="Z32" s="2"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
+      <c r="A33" s="5">
+        <v>545391.0</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="H33" s="5">
+        <v>9.987654326E9</v>
+      </c>
+      <c r="I33" s="10">
+        <f>DATE(2005,4,21)</f>
+        <v>38463</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="K33" s="2"/>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
@@ -1789,16 +2336,37 @@
       <c r="Z33" s="2"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
+      <c r="A34" s="5">
+        <v>534812.0</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="H34" s="5">
+        <v>9.234567819E9</v>
+      </c>
+      <c r="I34" s="10">
+        <f>DATE(2004,7,15)</f>
+        <v>38183</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="K34" s="2"/>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
@@ -1814,16 +2382,37 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
+      <c r="A35" s="5">
+        <v>554099.0</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G35" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="H35" s="5">
+        <v>9.456789014E9</v>
+      </c>
+      <c r="I35" s="10">
+        <f t="shared" ref="I35:I36" si="3">DATE(2002,2,17)</f>
+        <v>37304</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="K35" s="2"/>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
@@ -1839,16 +2428,37 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
+      <c r="A36" s="5">
+        <v>521763.0</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G36" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="H36" s="5">
+        <v>9.194567823E9</v>
+      </c>
+      <c r="I36" s="10">
+        <f t="shared" si="3"/>
+        <v>37304</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="K36" s="2"/>
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
@@ -1864,16 +2474,37 @@
       <c r="Z36" s="2"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
+      <c r="A37" s="5">
+        <v>525390.0</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="H37" s="5">
+        <v>9.213456789E9</v>
+      </c>
+      <c r="I37" s="10">
+        <f>DATE(2001,11,21)</f>
+        <v>37216</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="K37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
@@ -1889,16 +2520,37 @@
       <c r="Z37" s="2"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
+      <c r="A38" s="5">
+        <v>534218.0</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G38" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="H38" s="5">
+        <v>9.185678901E9</v>
+      </c>
+      <c r="I38" s="10">
+        <f>DATE(2002,1,12)</f>
+        <v>37268</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="K38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
@@ -1914,16 +2566,37 @@
       <c r="Z38" s="2"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
+      <c r="A39" s="5">
+        <v>522647.0</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G39" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="H39" s="5">
+        <v>9.182345678E9</v>
+      </c>
+      <c r="I39" s="10">
+        <f>DATE(2002,6,22)</f>
+        <v>37429</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="K39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
@@ -1939,16 +2612,37 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
+      <c r="A40" s="5">
+        <v>541837.0</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="H40" s="5">
+        <v>9.215678901E9</v>
+      </c>
+      <c r="I40" s="10">
+        <f>DATE(2005,10,8)</f>
+        <v>38633</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="K40" s="2"/>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
@@ -1964,16 +2658,37 @@
       <c r="Z40" s="2"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
+      <c r="A41" s="5">
+        <v>525390.0</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G41" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="H41" s="5">
+        <v>9.213456789E9</v>
+      </c>
+      <c r="I41" s="10">
+        <f>DATE(2001,12,1)</f>
+        <v>37226</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="K41" s="2"/>
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
@@ -1989,16 +2704,37 @@
       <c r="Z41" s="2"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
+      <c r="A42" s="5">
+        <v>545524.0</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="H42" s="8">
+        <v>9.630631698E9</v>
+      </c>
+      <c r="I42" s="11">
+        <f>DATE(2005,5,10)</f>
+        <v>38482</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="K42" s="2"/>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
@@ -2014,16 +2750,37 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
+      <c r="A43" s="5">
+        <v>543519.0</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="H43" s="5">
+        <v>9.77079601E9</v>
+      </c>
+      <c r="I43" s="11">
+        <f>DATE(2004,5,19)</f>
+        <v>38126</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="K43" s="2"/>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
@@ -25963,6 +26720,31 @@
       <c r="Y1000" s="2"/>
       <c r="Z1000" s="2"/>
     </row>
+    <row r="1001" ht="14.25" customHeight="1">
+      <c r="A1001" s="2"/>
+      <c r="B1001" s="2"/>
+      <c r="C1001" s="2"/>
+      <c r="D1001" s="2"/>
+      <c r="E1001" s="2"/>
+      <c r="F1001" s="2"/>
+      <c r="G1001" s="2"/>
+      <c r="H1001" s="2"/>
+      <c r="I1001" s="2"/>
+      <c r="J1001" s="2"/>
+      <c r="K1001" s="2"/>
+      <c r="O1001" s="2"/>
+      <c r="P1001" s="2"/>
+      <c r="Q1001" s="2"/>
+      <c r="R1001" s="2"/>
+      <c r="S1001" s="2"/>
+      <c r="T1001" s="2"/>
+      <c r="U1001" s="2"/>
+      <c r="V1001" s="2"/>
+      <c r="W1001" s="2"/>
+      <c r="X1001" s="2"/>
+      <c r="Y1001" s="2"/>
+      <c r="Z1001" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="E2"/>

</xml_diff>